<commit_message>
Data analysis | Histogram added
</commit_message>
<xml_diff>
--- a/data_analysis/data_analysis.xlsx
+++ b/data_analysis/data_analysis.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\river\OneDrive - Radboud Universiteit\Documenten\GitHub\thesis_face_gesture_project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6287B4B9-4F48-4EFA-A2AA-AC7B1EF39055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B59CE78-7E82-4C2D-A76C-AB64261757C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="3" r:id="rId1"/>
-    <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Individuales" sheetId="2" r:id="rId3"/>
-    <sheet name="Combinado" sheetId="4" r:id="rId4"/>
+    <sheet name="Accuracy" sheetId="5" r:id="rId2"/>
+    <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Individuales" sheetId="2" r:id="rId4"/>
+    <sheet name="Combinado" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -343,13 +344,32 @@
   <si>
     <t>ID_011</t>
   </si>
+  <si>
+    <t>System A Attempts</t>
+  </si>
+  <si>
+    <t>System A Successes</t>
+  </si>
+  <si>
+    <t>System B Attempts</t>
+  </si>
+  <si>
+    <t>System B Successes</t>
+  </si>
+  <si>
+    <t>System A Accuracy</t>
+  </si>
+  <si>
+    <t>System B Accuracy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -588,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -645,6 +665,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,8 +948,8 @@
   </sheetPr>
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2072,6 +2098,767 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AFCD81-EF32-4AF8-B34A-B3D6837D3930}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AE27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="19" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="6.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="13">
+        <v>5</v>
+      </c>
+      <c r="C2" s="20">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13">
+        <v>5</v>
+      </c>
+      <c r="E2" s="20">
+        <v>3</v>
+      </c>
+      <c r="F2" s="25">
+        <f>C2/B2</f>
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="26">
+        <f>E2/D2</f>
+        <v>0.6</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="20"/>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3" s="20">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13">
+        <v>6</v>
+      </c>
+      <c r="E3" s="20">
+        <v>4</v>
+      </c>
+      <c r="F3" s="25">
+        <f t="shared" ref="F3:F12" si="0">C3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="26">
+        <f t="shared" ref="G3:G12" si="1">E3/D3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="20"/>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="13">
+        <v>3</v>
+      </c>
+      <c r="C4" s="20">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13">
+        <v>5</v>
+      </c>
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="F4" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="20"/>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="13">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13">
+        <v>5</v>
+      </c>
+      <c r="E5" s="20">
+        <v>3</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="26">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="20"/>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5</v>
+      </c>
+      <c r="E6" s="20">
+        <v>4</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G6" s="26">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="20"/>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="13">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13">
+        <v>7</v>
+      </c>
+      <c r="E7" s="20">
+        <v>4</v>
+      </c>
+      <c r="F7" s="25">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="G7" s="26">
+        <f t="shared" si="1"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="20"/>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="13">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20">
+        <v>3</v>
+      </c>
+      <c r="D8" s="13">
+        <v>5</v>
+      </c>
+      <c r="E8" s="20">
+        <v>3</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="G8" s="26">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="20"/>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="20">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>3</v>
+      </c>
+      <c r="E9" s="20">
+        <v>2</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="26">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="20"/>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="13">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20">
+        <v>3</v>
+      </c>
+      <c r="D10" s="13">
+        <v>4</v>
+      </c>
+      <c r="E10" s="20">
+        <v>3</v>
+      </c>
+      <c r="F10" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="26">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="20"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="13">
+        <v>3</v>
+      </c>
+      <c r="C11" s="20">
+        <v>2</v>
+      </c>
+      <c r="D11" s="13">
+        <v>5</v>
+      </c>
+      <c r="E11" s="20">
+        <v>4</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G11" s="26">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="20"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="13">
+        <v>3</v>
+      </c>
+      <c r="C12" s="20">
+        <v>3</v>
+      </c>
+      <c r="D12" s="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="20">
+        <v>4</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="26">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="20"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="1:31" ht="13" x14ac:dyDescent="0.3">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="22"/>
+    </row>
+    <row r="17" spans="3:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21"/>
+      <c r="AE17" s="21"/>
+    </row>
+    <row r="18" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AE18" s="21"/>
+    </row>
+    <row r="19" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AE19" s="21"/>
+    </row>
+    <row r="20" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AE20" s="21"/>
+    </row>
+    <row r="21" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="21"/>
+      <c r="AE21" s="21"/>
+    </row>
+    <row r="22" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21"/>
+      <c r="AE22" s="21"/>
+    </row>
+    <row r="23" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+      <c r="AE23" s="21"/>
+    </row>
+    <row r="24" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AE24" s="21"/>
+    </row>
+    <row r="25" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AE25" s="21"/>
+    </row>
+    <row r="26" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AE26" s="21"/>
+    </row>
+    <row r="27" spans="3:31" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AE27" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2740,7 +3527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10425,7 +11212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>